<commit_message>
fix: reporte codigo proceso sw
</commit_message>
<xml_diff>
--- a/boot/src/main/resources/xlsx/mantenimientosgenerales/codigoProcesoSwitch.xlsx
+++ b/boot/src/main/resources/xlsx/mantenimientosgenerales/codigoProcesoSwitch.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14490" windowHeight="2580"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>&lt;jx:forEach items="${mantenimiento}" var="item" &gt;</t>
   </si>
@@ -51,18 +52,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Código Proceso Switch</t>
-  </si>
-  <si>
-    <t>${item.idCodigoProcesoSwitch} - ${item.abreviatura}</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>${item.descripcionCodigoProcesoSwitch}</t>
-  </si>
-  <si>
     <t>Abreviatura</t>
   </si>
   <si>
@@ -94,12 +83,18 @@
   </si>
   <si>
     <t>REPORTE DE CÓDIGO DE PROCESO SWITCH</t>
+  </si>
+  <si>
+    <t>${item.idCodigoProcesoSwitch} - ${item.descripcionCodProcesoSwitch}</t>
+  </si>
+  <si>
+    <t>Proceso Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -323,14 +318,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -363,18 +352,27 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -383,15 +381,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -727,56 +716,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
-    <col min="5" max="6" width="36.5703125" customWidth="1"/>
-    <col min="7" max="7" width="67.140625" customWidth="1"/>
-    <col min="8" max="8" width="62.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" customWidth="1"/>
-    <col min="10" max="10" width="39" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="22.5703125" customWidth="1"/>
-    <col min="13" max="13" width="33.28515625" customWidth="1"/>
-    <col min="14" max="14" width="37" customWidth="1"/>
-    <col min="15" max="15" width="64.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" customWidth="1"/>
+    <col min="6" max="6" width="67.140625" customWidth="1"/>
+    <col min="7" max="7" width="62.42578125" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="39" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="22.5703125" customWidth="1"/>
+    <col min="12" max="12" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="37" customWidth="1"/>
+    <col min="14" max="14" width="64.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:24" x14ac:dyDescent="0.25">
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
     </row>
     <row r="3" spans="3:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="18"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="3:24" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="29" t="s">
@@ -786,177 +774,166 @@
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
       <c r="O4" s="16"/>
-      <c r="P4" s="18"/>
     </row>
     <row r="5" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
-      <c r="D5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18"/>
+      <c r="D5" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
     </row>
     <row r="6" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="28"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
     </row>
     <row r="7" spans="3:24" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>
       <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="G7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="H7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="I7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="14"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="11"/>
+      <c r="V7" s="11"/>
+      <c r="W7" s="12"/>
     </row>
     <row r="8" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="3"/>
       <c r="D8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
     </row>
     <row r="9" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="4"/>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="I9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="15"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
     </row>
     <row r="10" spans="3:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+    </row>
+    <row r="18" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D5:J6"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="D5:I6"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>